<commit_message>
++ update làm trong khi check final += genera des
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/LogisticsImportChargeTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/LogisticsImportChargeTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.an\Desktop\eFMS\WebAPI\eFMS.API.SystemWeb\eFMS.API.Documentation\eFMS.API.Documentation\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynne.loc\Desktop\eFMSSource\WebAPI\eFMS.API.SystemWeb\eFMS.API.Documentation\eFMS.API.Documentation\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Custom No</t>
   </si>
@@ -258,6 +258,12 @@
       </rPr>
       <t>(*)</t>
     </r>
+  </si>
+  <si>
+    <t>OBH Partner</t>
+  </si>
+  <si>
+    <t>26784508</t>
   </si>
 </sst>
 </file>
@@ -636,30 +642,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -673,46 +678,49 @@
         <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -726,42 +734,45 @@
         <v>2342342</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8">
+      <c r="I2" s="8">
         <v>1000000</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>10</v>
       </c>
-      <c r="K2" s="9">
+      <c r="L2" s="9">
         <v>44210</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>23270</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="9">
+      <c r="O2" s="9">
         <v>44210</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
++column vatpartner into tmplate & info vatpartner
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/LogisticsImportChargeTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/LogisticsImportChargeTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynne.loc\Desktop\eFMSSource\WebAPI\eFMS.API.SystemWeb\eFMS.API.Documentation\eFMS.API.Documentation\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.Documentation\eFMS.API.Documentation\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Custom No</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>26784508</t>
+  </si>
+  <si>
+    <t>VAT Partner</t>
   </si>
 </sst>
 </file>
@@ -642,29 +645,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -696,31 +702,34 @@
         <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -751,28 +760,29 @@
       <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="L2" s="9">
+      <c r="M2" s="9">
         <v>44210</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>23270</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <v>44210</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prod/18953 add vat partner into import charge function job ops
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/LogisticsImportChargeTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/LogisticsImportChargeTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynne.loc\Desktop\eFMSSource\WebAPI\eFMS.API.SystemWeb\eFMS.API.Documentation\eFMS.API.Documentation\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.Documentation\eFMS.API.Documentation\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Custom No</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>26784508</t>
+  </si>
+  <si>
+    <t>VAT Partner</t>
   </si>
 </sst>
 </file>
@@ -642,29 +645,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -696,31 +702,34 @@
         <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -751,28 +760,29 @@
       <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="L2" s="9">
+      <c r="M2" s="9">
         <v>44210</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>23270</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <v>44210</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>